<commit_message>
Modified table for quote
</commit_message>
<xml_diff>
--- a/BOM_Connectors.xlsx
+++ b/BOM_Connectors.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Files\GenInfy\PCB Designs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Files\GenInfy\PCB Designs\SB_Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA1144B-00A1-4AAF-97A7-A4F643A4806F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B751A429-806A-4257-B0C7-6C2F62466DDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7305" windowWidth="29040" windowHeight="15840" xr2:uid="{B2FF7981-B026-4E72-8265-FA2A917B3FE0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
   <si>
     <t>S.No</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Quantity</t>
-  </si>
-  <si>
     <t>Reference</t>
   </si>
   <si>
@@ -51,9 +48,6 @@
     <t>Pitch 2MM, 4POS, VERTICAL CONNECTOR</t>
   </si>
   <si>
-    <t>Female to Female cable for connector above</t>
-  </si>
-  <si>
     <t>440055-4</t>
   </si>
   <si>
@@ -90,24 +84,6 @@
     <t>Pitch 2.5MM, 2POS, VERTICAL CONNECTOR</t>
   </si>
   <si>
-    <t>https://www.te.com/usa-en/product-1776119-3.html</t>
-  </si>
-  <si>
-    <t>1776119-3</t>
-  </si>
-  <si>
-    <t>Screw Terminal Pitch 5.08MM, 3POS</t>
-  </si>
-  <si>
-    <t>https://www.te.com/usa-en/product-1546217-2.html</t>
-  </si>
-  <si>
-    <t>Screw Terminal Pitch 5.08MM, 2POS</t>
-  </si>
-  <si>
-    <t>1546217-2</t>
-  </si>
-  <si>
     <t>https://www.te.com/usa-en/product-103311-5.html</t>
   </si>
   <si>
@@ -133,6 +109,54 @@
   </si>
   <si>
     <t>https://www.te.com/global-en/product-1-1612962-3.html</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>3v3</t>
+  </si>
+  <si>
+    <t>50mA</t>
+  </si>
+  <si>
+    <t>Connecting to end stop Limit Switch module</t>
+  </si>
+  <si>
+    <t>Connecting to end stop Tactile Switch module</t>
+  </si>
+  <si>
+    <t>Connecting to end stop Limit Switch module with LED</t>
+  </si>
+  <si>
+    <t>100mA</t>
+  </si>
+  <si>
+    <t>Water Pump</t>
+  </si>
+  <si>
+    <t>12v</t>
+  </si>
+  <si>
+    <t>0.5A</t>
+  </si>
+  <si>
+    <t>Max. Voltage</t>
+  </si>
+  <si>
+    <t>Max. Current</t>
+  </si>
+  <si>
+    <t>12V</t>
+  </si>
+  <si>
+    <t>2A</t>
+  </si>
+  <si>
+    <t>Power and Signals</t>
+  </si>
+  <si>
+    <t>24V</t>
   </si>
 </sst>
 </file>
@@ -185,12 +209,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -510,18 +531,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C49E823-9816-4E79-8A36-8C80C67ABCEA}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
     <col min="3" max="3" width="39" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="48.77734375" customWidth="1"/>
+    <col min="4" max="4" width="52.21875" customWidth="1"/>
+    <col min="5" max="5" width="50.109375" customWidth="1"/>
     <col min="6" max="6" width="22.44140625" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
   </cols>
@@ -540,250 +561,211 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2">
-        <v>50</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>5</v>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2">
-        <v>20</v>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2">
-        <v>50</v>
-      </c>
-      <c r="E4" s="4" t="s">
         <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
       <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>12</v>
+      <c r="B6" t="s">
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="2">
-        <v>10</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="2">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="2">
-        <v>10</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="2">
-        <v>50</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="2">
-        <v>20</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="2">
-        <v>20</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="2">
-        <v>10</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="2">
-        <v>10</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="2">
-        <v>10</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>34</v>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E15" r:id="rId1" xr:uid="{3CD3FA61-22F3-4E89-A074-F15F27EDF3D4}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{C244CF03-F903-4F2A-97FE-15F40A1180D0}"/>
-    <hyperlink ref="E14" r:id="rId3" xr:uid="{AB7C4269-03D2-4491-A027-F402A44CC6FA}"/>
-    <hyperlink ref="E13" r:id="rId4" xr:uid="{3E0E155D-CF59-4389-A468-981A3E878996}"/>
-    <hyperlink ref="E4" r:id="rId5" xr:uid="{B543C60E-9F8A-444F-8240-C9C8F728FE3F}"/>
-    <hyperlink ref="E6" r:id="rId6" xr:uid="{7A06ED1E-D5C8-472E-B8DA-E6B5863A3C48}"/>
-    <hyperlink ref="E8" r:id="rId7" xr:uid="{174AD484-03E0-44CB-90A3-EDD0CC1DD130}"/>
-    <hyperlink ref="E10" r:id="rId8" xr:uid="{FCB0D743-C235-46CD-B94B-DFE8C7945518}"/>
-    <hyperlink ref="E12" r:id="rId9" xr:uid="{6654A82B-A1E0-4845-9278-B8C923AAC0FF}"/>
-    <hyperlink ref="E16" r:id="rId10" xr:uid="{78EFA096-276B-4A8A-8BFF-3638D0D62B18}"/>
+    <hyperlink ref="D8" r:id="rId1" xr:uid="{3CD3FA61-22F3-4E89-A074-F15F27EDF3D4}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{C244CF03-F903-4F2A-97FE-15F40A1180D0}"/>
+    <hyperlink ref="D7" r:id="rId3" xr:uid="{AB7C4269-03D2-4491-A027-F402A44CC6FA}"/>
+    <hyperlink ref="D3" r:id="rId4" xr:uid="{B543C60E-9F8A-444F-8240-C9C8F728FE3F}"/>
+    <hyperlink ref="D4" r:id="rId5" xr:uid="{7A06ED1E-D5C8-472E-B8DA-E6B5863A3C48}"/>
+    <hyperlink ref="D5" r:id="rId6" xr:uid="{174AD484-03E0-44CB-90A3-EDD0CC1DD130}"/>
+    <hyperlink ref="D6" r:id="rId7" xr:uid="{FCB0D743-C235-46CD-B94B-DFE8C7945518}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{78EFA096-276B-4A8A-8BFF-3638D0D62B18}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>